<commit_message>
incorporacion de irradiancia iv600
</commit_message>
<xml_diff>
--- a/pvstand/datos_procesados_analisis_integrado_py/iv600/iv_curves/iv_curves_report.xlsx
+++ b/pvstand/datos_procesados_analisis_integrado_py/iv600/iv_curves/iv_curves_report.xlsx
@@ -472,7 +472,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -490,13 +490,15 @@
           <t>IV600</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>725</v>
+      </c>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -514,13 +516,15 @@
           <t>IV600</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>725</v>
+      </c>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -538,7 +542,9 @@
           <t>IV600</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>725</v>
+      </c>
       <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
@@ -635,7 +641,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -648,7 +654,9 @@
           <t>IV600_sample_1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>725</v>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>380.686889648438</v>
@@ -678,7 +686,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -691,7 +699,9 @@
           <t>IV600_sample_2</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>725</v>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>380.693603515625</v>
@@ -721,7 +731,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -734,7 +744,9 @@
           <t>IV600_sample_3</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>725</v>
+      </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>315.244567871094</v>

</xml_diff>

<commit_message>
incorporacion de curvas del 04/11/2025
</commit_message>
<xml_diff>
--- a/pvstand/datos_procesados_analisis_integrado_py/iv600/iv_curves/iv_curves_report.xlsx
+++ b/pvstand/datos_procesados_analisis_integrado_py/iv600/iv_curves/iv_curves_report.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-11-07</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-11-07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-11-07</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>